<commit_message>
Worked on Levels, changed the soundsystem -> it works on a single thread now.
</commit_message>
<xml_diff>
--- a/LayoutLevel.xlsx
+++ b/LayoutLevel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog4Engine\minigin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64EEF87C-DE36-4C98-81CE-147B6EAB297F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165ED5A2-49F3-4C48-80E7-D98CF5B0AB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="11910" windowWidth="19200" windowHeight="9090" xr2:uid="{B0A83D7C-9DD1-4CD4-A1ED-75D0E3A69170}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="10500" xr2:uid="{B0A83D7C-9DD1-4CD4-A1ED-75D0E3A69170}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>spawning</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -54,7 +57,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -64,6 +67,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -95,10 +128,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -413,11 +454,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D9F4A7-31DE-4023-B813-576E506462B3}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:AR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -436,139 +475,269 @@
     <col min="13" max="16" width="5.140625" customWidth="1"/>
     <col min="17" max="17" width="4.85546875" customWidth="1"/>
     <col min="18" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="4.140625" customWidth="1"/>
-    <col min="20" max="20" width="4.5703125" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" customWidth="1"/>
+    <col min="22" max="23" width="5.7109375" customWidth="1"/>
+    <col min="24" max="30" width="3.7109375" customWidth="1"/>
+    <col min="31" max="36" width="4.7109375" customWidth="1"/>
+    <col min="37" max="37" width="5.7109375" customWidth="1"/>
+    <col min="38" max="38" width="4.28515625" customWidth="1"/>
+    <col min="39" max="39" width="5.85546875" customWidth="1"/>
+    <col min="40" max="40" width="5.7109375" customWidth="1"/>
+    <col min="41" max="41" width="5.28515625" customWidth="1"/>
+    <col min="42" max="42" width="4.85546875" customWidth="1"/>
+    <col min="43" max="43" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
+    <row r="1" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="7">
         <v>15</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="7">
         <v>29</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="7">
         <v>43</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="7">
         <v>57</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="7">
         <v>71</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="7">
         <v>85</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="7">
         <v>99</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="7">
         <v>113</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="7">
         <v>127</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="7">
         <v>141</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="7">
         <v>155</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M1" s="7">
         <v>169</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1" s="7">
         <v>183</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="7">
         <v>197</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="7">
         <v>211</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="7">
         <v>225</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1" s="7">
         <v>239</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S1" s="7">
         <v>253</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T1" s="7">
         <v>267</v>
       </c>
+      <c r="X1" s="7">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="7">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="7">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="7">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="7">
+        <v>71</v>
+      </c>
+      <c r="AD1" s="7">
+        <v>85</v>
+      </c>
+      <c r="AE1" s="7">
+        <v>99</v>
+      </c>
+      <c r="AF1" s="7">
+        <v>113</v>
+      </c>
+      <c r="AG1" s="7">
+        <v>127</v>
+      </c>
+      <c r="AH1" s="7">
+        <v>141</v>
+      </c>
+      <c r="AI1" s="7">
+        <v>155</v>
+      </c>
+      <c r="AJ1" s="7">
+        <v>169</v>
+      </c>
+      <c r="AK1" s="7">
+        <v>183</v>
+      </c>
+      <c r="AL1" s="7">
+        <v>197</v>
+      </c>
+      <c r="AM1" s="7">
+        <v>211</v>
+      </c>
+      <c r="AN1" s="7">
+        <v>225</v>
+      </c>
+      <c r="AO1" s="7">
+        <v>239</v>
+      </c>
+      <c r="AP1" s="7">
+        <v>253</v>
+      </c>
+      <c r="AQ1" s="7">
+        <v>267</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="7">
         <v>16</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="7">
         <v>30</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="7">
         <v>44</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="7">
         <v>58</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="7">
         <v>72</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="7">
         <v>86</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="7">
         <v>100</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="7">
         <v>114</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="7">
         <v>128</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="7">
         <v>142</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="7">
         <v>156</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="7">
         <v>170</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="7">
         <v>184</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="7">
         <v>198</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="7">
         <v>212</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2" s="7">
         <v>226</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="7">
         <v>240</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="7">
         <v>254</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T2" s="7">
         <v>268</v>
       </c>
+      <c r="X2" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>16</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>58</v>
+      </c>
+      <c r="AC2" s="7">
+        <v>72</v>
+      </c>
+      <c r="AD2" s="7">
+        <v>86</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>100</v>
+      </c>
+      <c r="AF2" s="7">
+        <v>114</v>
+      </c>
+      <c r="AG2" s="7">
+        <v>128</v>
+      </c>
+      <c r="AH2" s="7">
+        <v>142</v>
+      </c>
+      <c r="AI2" s="7">
+        <v>156</v>
+      </c>
+      <c r="AJ2" s="7">
+        <v>170</v>
+      </c>
+      <c r="AK2" s="7">
+        <v>184</v>
+      </c>
+      <c r="AL2" s="7">
+        <v>198</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>212</v>
+      </c>
+      <c r="AN2" s="7">
+        <v>226</v>
+      </c>
+      <c r="AO2" s="7">
+        <v>240</v>
+      </c>
+      <c r="AP2" s="7">
+        <v>254</v>
+      </c>
+      <c r="AQ2" s="7">
+        <v>268</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>17</v>
       </c>
       <c r="C3" s="1">
@@ -577,125 +746,248 @@
       <c r="D3" s="1">
         <v>45</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>59</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>73</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="6">
         <v>87</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>101</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <v>115</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="3">
         <v>129</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="3">
         <v>143</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="6">
         <v>157</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="3">
         <v>171</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="3">
         <v>185</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="3">
         <v>199</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="3">
         <v>213</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="3">
         <v>227</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="3">
         <v>241</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="3">
         <v>255</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="3">
         <v>269</v>
       </c>
-      <c r="U3" t="s">
-        <v>0</v>
+      <c r="X3" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>17</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>59</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>73</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>87</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>101</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>115</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>129</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>143</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>157</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>171</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>185</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>199</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>213</v>
+      </c>
+      <c r="AN3" s="3">
+        <v>227</v>
+      </c>
+      <c r="AO3" s="10">
+        <v>241</v>
+      </c>
+      <c r="AP3" s="3">
+        <v>255</v>
+      </c>
+      <c r="AQ3" s="3">
+        <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>18</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>32</v>
       </c>
       <c r="D4" s="1">
         <v>46</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>60</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>74</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="4">
         <v>88</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>102</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3">
         <v>116</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="3">
         <v>130</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="4">
         <v>144</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="3">
         <v>158</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="3">
         <v>172</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="2">
         <v>186</v>
       </c>
       <c r="O4" s="2">
         <v>200</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="2">
         <v>214</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="2">
         <v>228</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="2">
         <v>242</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="2">
         <v>256</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4" s="2">
         <v>270</v>
       </c>
+      <c r="U4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" s="4">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>18</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="10">
+        <v>46</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>60</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>74</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>88</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>102</v>
+      </c>
+      <c r="AF4" s="10">
+        <v>116</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>130</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>144</v>
+      </c>
+      <c r="AI4" s="4">
+        <v>158</v>
+      </c>
+      <c r="AJ4" s="4">
+        <v>172</v>
+      </c>
+      <c r="AK4" s="10">
+        <v>186</v>
+      </c>
+      <c r="AL4" s="3">
+        <v>200</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>214</v>
+      </c>
+      <c r="AN4" s="3">
+        <v>228</v>
+      </c>
+      <c r="AO4" s="3">
+        <v>242</v>
+      </c>
+      <c r="AP4" s="3">
+        <v>256</v>
+      </c>
+      <c r="AQ4" s="2">
+        <v>270</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>19</v>
       </c>
       <c r="C5" s="1">
@@ -704,60 +996,120 @@
       <c r="D5" s="1">
         <v>47</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>61</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="4">
         <v>75</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>89</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>103</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
         <v>117</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3">
         <v>131</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="4">
         <v>145</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>159</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="3">
         <v>173</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="2">
         <v>187</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="3">
         <v>201</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="3">
         <v>215</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="6">
         <v>229</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="3">
         <v>243</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="3">
         <v>257</v>
       </c>
-      <c r="T5" s="1">
+      <c r="T5" s="3">
         <v>271</v>
       </c>
+      <c r="X5" s="4">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>33</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>47</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>61</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>75</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>89</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>103</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>117</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>131</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>145</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>159</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>173</v>
+      </c>
+      <c r="AK5" s="3">
+        <v>187</v>
+      </c>
+      <c r="AL5" s="3">
+        <v>201</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>215</v>
+      </c>
+      <c r="AN5" s="3">
+        <v>229</v>
+      </c>
+      <c r="AO5" s="3">
+        <v>243</v>
+      </c>
+      <c r="AP5" s="3">
+        <v>257</v>
+      </c>
+      <c r="AQ5" s="2">
+        <v>271</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>20</v>
       </c>
       <c r="C6" s="1">
@@ -766,60 +1118,120 @@
       <c r="D6" s="1">
         <v>48</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>62</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>76</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>90</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>104</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="3">
         <v>118</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <v>132</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="4">
         <v>146</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="3">
         <v>160</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="3">
         <v>174</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="2">
         <v>188</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="3">
         <v>202</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="3">
         <v>216</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="3">
         <v>230</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="3">
         <v>244</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="3">
         <v>258</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="3">
         <v>272</v>
       </c>
+      <c r="X6" s="4">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>20</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>48</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>62</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>76</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>90</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>104</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>118</v>
+      </c>
+      <c r="AG6" s="4">
+        <v>132</v>
+      </c>
+      <c r="AH6" s="4">
+        <v>146</v>
+      </c>
+      <c r="AI6" s="4">
+        <v>160</v>
+      </c>
+      <c r="AJ6" s="4">
+        <v>174</v>
+      </c>
+      <c r="AK6" s="3">
+        <v>188</v>
+      </c>
+      <c r="AL6" s="3">
+        <v>202</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>216</v>
+      </c>
+      <c r="AN6" s="3">
+        <v>230</v>
+      </c>
+      <c r="AO6" s="3">
+        <v>244</v>
+      </c>
+      <c r="AP6" s="3">
+        <v>258</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>272</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>21</v>
       </c>
       <c r="C7" s="1">
@@ -828,242 +1240,482 @@
       <c r="D7" s="1">
         <v>49</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>63</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>77</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>91</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>105</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="3">
         <v>119</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="3">
         <v>133</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="4">
         <v>147</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="3">
         <v>161</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3">
         <v>175</v>
       </c>
       <c r="N7" s="2">
         <v>189</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="3">
         <v>203</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="4">
         <v>217</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="4">
         <v>231</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="4">
         <v>245</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="3">
         <v>259</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T7" s="3">
         <v>273</v>
       </c>
+      <c r="X7" s="3">
+        <v>7</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>21</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>35</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>49</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>63</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>77</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>91</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>105</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>119</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>133</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>147</v>
+      </c>
+      <c r="AI7" s="3">
+        <v>161</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>175</v>
+      </c>
+      <c r="AK7" s="3">
+        <v>189</v>
+      </c>
+      <c r="AL7" s="3">
+        <v>203</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>217</v>
+      </c>
+      <c r="AN7" s="3">
+        <v>231</v>
+      </c>
+      <c r="AO7" s="3">
+        <v>245</v>
+      </c>
+      <c r="AP7" s="3">
+        <v>259</v>
+      </c>
+      <c r="AQ7" s="2">
+        <v>273</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>22</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>36</v>
       </c>
       <c r="D8" s="1">
         <v>50</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>64</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>78</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>92</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>106</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>120</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="6">
         <v>134</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="4">
         <v>148</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="3">
         <v>162</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="3">
         <v>176</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="2">
         <v>190</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="3">
         <v>204</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="4">
         <v>218</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="4">
         <v>232</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="4">
         <v>246</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="3">
         <v>260</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8" s="3">
         <v>274</v>
       </c>
+      <c r="X8" s="3">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>22</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>50</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>64</v>
+      </c>
+      <c r="AC8" s="4">
+        <v>78</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>92</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>106</v>
+      </c>
+      <c r="AF8" s="10">
+        <v>120</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>134</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>148</v>
+      </c>
+      <c r="AI8" s="4">
+        <v>162</v>
+      </c>
+      <c r="AJ8" s="4">
+        <v>176</v>
+      </c>
+      <c r="AK8" s="10">
+        <v>190</v>
+      </c>
+      <c r="AL8" s="3">
+        <v>204</v>
+      </c>
+      <c r="AM8" s="2">
+        <v>218</v>
+      </c>
+      <c r="AN8" s="3">
+        <v>232</v>
+      </c>
+      <c r="AO8" s="3">
+        <v>246</v>
+      </c>
+      <c r="AP8" s="3">
+        <v>260</v>
+      </c>
+      <c r="AQ8" s="2">
+        <v>274</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>23</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>37</v>
       </c>
       <c r="D9" s="1">
         <v>51</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>65</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>79</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
         <v>93</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>107</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>121</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="3">
         <v>135</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="3">
         <v>149</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="6">
         <v>163</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="3">
         <v>177</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="2">
         <v>191</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="3">
         <v>205</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="3">
         <v>219</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="3">
         <v>233</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="3">
         <v>247</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="3">
         <v>261</v>
       </c>
-      <c r="T9" s="1">
+      <c r="T9" s="3">
         <v>275</v>
       </c>
+      <c r="X9" s="3">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>23</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>37</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>51</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>65</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>79</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>93</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>107</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>121</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>135</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>149</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>163</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>177</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>191</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>205</v>
+      </c>
+      <c r="AM9" s="2">
+        <v>219</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>233</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>247</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>261</v>
+      </c>
+      <c r="AQ9" s="2">
+        <v>275</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>24</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>38</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>52</v>
       </c>
       <c r="E10" s="2">
         <v>66</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>80</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>94</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>108</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>122</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="3">
         <v>136</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="3">
         <v>150</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="3">
         <v>164</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="3">
         <v>178</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="2">
         <v>192</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O10" s="3">
         <v>206</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="3">
         <v>220</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10" s="4">
         <v>234</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="4">
         <v>248</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="4">
         <v>262</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10" s="3">
         <v>276</v>
       </c>
+      <c r="X10" s="3">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>24</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>38</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>52</v>
+      </c>
+      <c r="AB10" s="4">
+        <v>66</v>
+      </c>
+      <c r="AC10" s="4">
+        <v>80</v>
+      </c>
+      <c r="AD10" s="4">
+        <v>94</v>
+      </c>
+      <c r="AE10" s="4">
+        <v>108</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>122</v>
+      </c>
+      <c r="AG10" s="4">
+        <v>136</v>
+      </c>
+      <c r="AH10" s="4">
+        <v>150</v>
+      </c>
+      <c r="AI10" s="4">
+        <v>164</v>
+      </c>
+      <c r="AJ10" s="4">
+        <v>178</v>
+      </c>
+      <c r="AK10" s="3">
+        <v>192</v>
+      </c>
+      <c r="AL10" s="3">
+        <v>206</v>
+      </c>
+      <c r="AM10" s="2">
+        <v>220</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>234</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>248</v>
+      </c>
+      <c r="AP10" s="3">
+        <v>262</v>
+      </c>
+      <c r="AQ10" s="2">
+        <v>276</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -1076,60 +1728,120 @@
       <c r="D11" s="1">
         <v>53</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>67</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>81</v>
       </c>
       <c r="G11" s="2">
         <v>95</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="3">
         <v>109</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <v>123</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="3">
         <v>137</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="3">
         <v>151</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="3">
         <v>165</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="3">
         <v>179</v>
       </c>
       <c r="N11" s="2">
         <v>193</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="3">
         <v>207</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="3">
         <v>221</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="4">
         <v>235</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="4">
         <v>249</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="4">
         <v>263</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T11" s="3">
         <v>277</v>
       </c>
+      <c r="X11" s="3">
+        <v>11</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>25</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>39</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>53</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>67</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>81</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>95</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>109</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>123</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>137</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>151</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>165</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>179</v>
+      </c>
+      <c r="AK11" s="3">
+        <v>193</v>
+      </c>
+      <c r="AL11" s="3">
+        <v>207</v>
+      </c>
+      <c r="AM11" s="2">
+        <v>221</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>235</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>249</v>
+      </c>
+      <c r="AP11" s="3">
+        <v>263</v>
+      </c>
+      <c r="AQ11" s="2">
+        <v>277</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>26</v>
       </c>
       <c r="C12" s="1">
@@ -1144,28 +1856,28 @@
       <c r="F12" s="1">
         <v>82</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>96</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>110</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2">
         <v>124</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
         <v>138</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
         <v>152</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="2">
         <v>166</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="2">
         <v>180</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="2">
         <v>194</v>
       </c>
       <c r="O12" s="1">
@@ -1186,15 +1898,75 @@
       <c r="T12" s="1">
         <v>278</v>
       </c>
+      <c r="X12" s="3">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>26</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>40</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>54</v>
+      </c>
+      <c r="AB12" s="4">
+        <v>68</v>
+      </c>
+      <c r="AC12" s="4">
+        <v>82</v>
+      </c>
+      <c r="AD12" s="4">
+        <v>96</v>
+      </c>
+      <c r="AE12" s="4">
+        <v>110</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>124</v>
+      </c>
+      <c r="AG12" s="4">
+        <v>138</v>
+      </c>
+      <c r="AH12" s="4">
+        <v>152</v>
+      </c>
+      <c r="AI12" s="4">
+        <v>166</v>
+      </c>
+      <c r="AJ12" s="4">
+        <v>180</v>
+      </c>
+      <c r="AK12" s="3">
+        <v>194</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>208</v>
+      </c>
+      <c r="AM12" s="2">
+        <v>222</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>236</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>250</v>
+      </c>
+      <c r="AP12" s="3">
+        <v>264</v>
+      </c>
+      <c r="AQ12" s="2">
+        <v>278</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>13</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="4">
         <v>27</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>41</v>
       </c>
       <c r="D13" s="1">
@@ -1242,14 +2014,74 @@
       <c r="R13" s="1">
         <v>251</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" s="4">
         <v>265</v>
       </c>
       <c r="T13" s="1">
         <v>279</v>
       </c>
+      <c r="X13" s="3">
+        <v>13</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>27</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>41</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>55</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>69</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>83</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>97</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>111</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>125</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>139</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>153</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>167</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>181</v>
+      </c>
+      <c r="AK13" s="3">
+        <v>195</v>
+      </c>
+      <c r="AL13" s="3">
+        <v>209</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>223</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>237</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>251</v>
+      </c>
+      <c r="AP13" s="3">
+        <v>265</v>
+      </c>
+      <c r="AQ13" s="2">
+        <v>279</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -1277,10 +2109,10 @@
       <c r="I14" s="1">
         <v>126</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="4">
         <v>140</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="4">
         <v>154</v>
       </c>
       <c r="L14" s="1">
@@ -1310,8 +2142,950 @@
       <c r="T14" s="1">
         <v>280</v>
       </c>
+      <c r="X14" s="3">
+        <v>14</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>28</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>42</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>56</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>70</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>84</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>98</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>112</v>
+      </c>
+      <c r="AF14" s="3">
+        <v>126</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>140</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>154</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>168</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>182</v>
+      </c>
+      <c r="AK14" s="3">
+        <v>196</v>
+      </c>
+      <c r="AL14" s="3">
+        <v>210</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>224</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>238</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>252</v>
+      </c>
+      <c r="AP14" s="2">
+        <v>266</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>280</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:44" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N17" s="5"/>
+      <c r="Z17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>1</v>
+      </c>
+      <c r="B19" s="7">
+        <v>15</v>
+      </c>
+      <c r="C19" s="7">
+        <v>29</v>
+      </c>
+      <c r="D19" s="7">
+        <v>43</v>
+      </c>
+      <c r="E19" s="7">
+        <v>57</v>
+      </c>
+      <c r="F19" s="7">
+        <v>71</v>
+      </c>
+      <c r="G19" s="7">
+        <v>85</v>
+      </c>
+      <c r="H19" s="7">
+        <v>99</v>
+      </c>
+      <c r="I19" s="7">
+        <v>113</v>
+      </c>
+      <c r="J19" s="7">
+        <v>127</v>
+      </c>
+      <c r="K19" s="7">
+        <v>141</v>
+      </c>
+      <c r="L19" s="7">
+        <v>155</v>
+      </c>
+      <c r="M19" s="7">
+        <v>169</v>
+      </c>
+      <c r="N19" s="7">
+        <v>183</v>
+      </c>
+      <c r="O19" s="7">
+        <v>197</v>
+      </c>
+      <c r="P19" s="7">
+        <v>211</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>225</v>
+      </c>
+      <c r="R19" s="7">
+        <v>239</v>
+      </c>
+      <c r="S19" s="7">
+        <v>253</v>
+      </c>
+      <c r="T19" s="7">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>2</v>
+      </c>
+      <c r="B20" s="7">
+        <v>16</v>
+      </c>
+      <c r="C20" s="7">
+        <v>30</v>
+      </c>
+      <c r="D20" s="7">
+        <v>44</v>
+      </c>
+      <c r="E20" s="7">
+        <v>58</v>
+      </c>
+      <c r="F20" s="7">
+        <v>72</v>
+      </c>
+      <c r="G20" s="7">
+        <v>86</v>
+      </c>
+      <c r="H20" s="7">
+        <v>100</v>
+      </c>
+      <c r="I20" s="7">
+        <v>114</v>
+      </c>
+      <c r="J20" s="7">
+        <v>128</v>
+      </c>
+      <c r="K20" s="7">
+        <v>142</v>
+      </c>
+      <c r="L20" s="7">
+        <v>156</v>
+      </c>
+      <c r="M20" s="7">
+        <v>170</v>
+      </c>
+      <c r="N20" s="7">
+        <v>184</v>
+      </c>
+      <c r="O20" s="7">
+        <v>198</v>
+      </c>
+      <c r="P20" s="7">
+        <v>212</v>
+      </c>
+      <c r="Q20" s="7">
+        <v>226</v>
+      </c>
+      <c r="R20" s="7">
+        <v>240</v>
+      </c>
+      <c r="S20" s="7">
+        <v>254</v>
+      </c>
+      <c r="T20" s="7">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2">
+        <v>17</v>
+      </c>
+      <c r="C21" s="2">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2">
+        <v>45</v>
+      </c>
+      <c r="E21" s="2">
+        <v>59</v>
+      </c>
+      <c r="F21" s="2">
+        <v>73</v>
+      </c>
+      <c r="G21" s="2">
+        <v>87</v>
+      </c>
+      <c r="H21" s="2">
+        <v>101</v>
+      </c>
+      <c r="I21" s="2">
+        <v>115</v>
+      </c>
+      <c r="J21" s="2">
+        <v>129</v>
+      </c>
+      <c r="K21" s="2">
+        <v>143</v>
+      </c>
+      <c r="L21" s="2">
+        <v>157</v>
+      </c>
+      <c r="M21" s="2">
+        <v>171</v>
+      </c>
+      <c r="N21" s="2">
+        <v>185</v>
+      </c>
+      <c r="O21" s="2">
+        <v>199</v>
+      </c>
+      <c r="P21" s="2">
+        <v>213</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>227</v>
+      </c>
+      <c r="R21" s="2">
+        <v>241</v>
+      </c>
+      <c r="S21" s="2">
+        <v>255</v>
+      </c>
+      <c r="T21" s="2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3">
+        <v>32</v>
+      </c>
+      <c r="D22" s="3">
+        <v>46</v>
+      </c>
+      <c r="E22" s="4">
+        <v>60</v>
+      </c>
+      <c r="F22" s="4">
+        <v>74</v>
+      </c>
+      <c r="G22" s="9">
+        <v>88</v>
+      </c>
+      <c r="H22" s="4">
+        <v>102</v>
+      </c>
+      <c r="I22" s="4">
+        <v>116</v>
+      </c>
+      <c r="J22" s="4">
+        <v>130</v>
+      </c>
+      <c r="K22" s="4">
+        <v>144</v>
+      </c>
+      <c r="L22" s="4">
+        <v>158</v>
+      </c>
+      <c r="M22" s="4">
+        <v>172</v>
+      </c>
+      <c r="N22" s="9">
+        <v>186</v>
+      </c>
+      <c r="O22" s="4">
+        <v>200</v>
+      </c>
+      <c r="P22" s="4">
+        <v>214</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>228</v>
+      </c>
+      <c r="R22" s="3">
+        <v>242</v>
+      </c>
+      <c r="S22" s="3">
+        <v>256</v>
+      </c>
+      <c r="T22" s="2">
+        <v>270</v>
+      </c>
+      <c r="U22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3">
+        <v>33</v>
+      </c>
+      <c r="D23" s="3">
+        <v>47</v>
+      </c>
+      <c r="E23" s="3">
+        <v>61</v>
+      </c>
+      <c r="F23" s="4">
+        <v>75</v>
+      </c>
+      <c r="G23" s="4">
+        <v>89</v>
+      </c>
+      <c r="H23" s="4">
+        <v>103</v>
+      </c>
+      <c r="I23" s="4">
+        <v>117</v>
+      </c>
+      <c r="J23" s="9">
+        <v>131</v>
+      </c>
+      <c r="K23" s="9">
+        <v>145</v>
+      </c>
+      <c r="L23" s="4">
+        <v>159</v>
+      </c>
+      <c r="M23" s="4">
+        <v>173</v>
+      </c>
+      <c r="N23" s="4">
+        <v>187</v>
+      </c>
+      <c r="O23" s="4">
+        <v>201</v>
+      </c>
+      <c r="P23" s="3">
+        <v>215</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>229</v>
+      </c>
+      <c r="R23" s="3">
+        <v>243</v>
+      </c>
+      <c r="S23" s="3">
+        <v>257</v>
+      </c>
+      <c r="T23" s="2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2">
+        <v>48</v>
+      </c>
+      <c r="E24" s="3">
+        <v>62</v>
+      </c>
+      <c r="F24" s="3">
+        <v>76</v>
+      </c>
+      <c r="G24" s="4">
+        <v>90</v>
+      </c>
+      <c r="H24" s="4">
+        <v>104</v>
+      </c>
+      <c r="I24" s="4">
+        <v>118</v>
+      </c>
+      <c r="J24" s="4">
+        <v>132</v>
+      </c>
+      <c r="K24" s="4">
+        <v>146</v>
+      </c>
+      <c r="L24" s="4">
+        <v>160</v>
+      </c>
+      <c r="M24" s="4">
+        <v>174</v>
+      </c>
+      <c r="N24" s="4">
+        <v>188</v>
+      </c>
+      <c r="O24" s="3">
+        <v>202</v>
+      </c>
+      <c r="P24" s="3">
+        <v>216</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>230</v>
+      </c>
+      <c r="R24" s="2">
+        <v>244</v>
+      </c>
+      <c r="S24" s="2">
+        <v>258</v>
+      </c>
+      <c r="T24" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3">
+        <v>21</v>
+      </c>
+      <c r="C25" s="9">
+        <v>35</v>
+      </c>
+      <c r="D25" s="2">
+        <v>49</v>
+      </c>
+      <c r="E25" s="3">
+        <v>63</v>
+      </c>
+      <c r="F25" s="3">
+        <v>77</v>
+      </c>
+      <c r="G25" s="3">
+        <v>91</v>
+      </c>
+      <c r="H25" s="3">
+        <v>105</v>
+      </c>
+      <c r="I25" s="3">
+        <v>119</v>
+      </c>
+      <c r="J25" s="3">
+        <v>133</v>
+      </c>
+      <c r="K25" s="3">
+        <v>147</v>
+      </c>
+      <c r="L25" s="3">
+        <v>161</v>
+      </c>
+      <c r="M25" s="3">
+        <v>175</v>
+      </c>
+      <c r="N25" s="3">
+        <v>189</v>
+      </c>
+      <c r="O25" s="3">
+        <v>203</v>
+      </c>
+      <c r="P25" s="3">
+        <v>217</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>231</v>
+      </c>
+      <c r="R25" s="9">
+        <v>245</v>
+      </c>
+      <c r="S25" s="3">
+        <v>259</v>
+      </c>
+      <c r="T25" s="2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4">
+        <v>36</v>
+      </c>
+      <c r="D26" s="2">
+        <v>50</v>
+      </c>
+      <c r="E26" s="2">
+        <v>64</v>
+      </c>
+      <c r="F26" s="2">
+        <v>78</v>
+      </c>
+      <c r="G26" s="3">
+        <v>92</v>
+      </c>
+      <c r="H26" s="3">
+        <v>106</v>
+      </c>
+      <c r="I26" s="3">
+        <v>120</v>
+      </c>
+      <c r="J26" s="3">
+        <v>134</v>
+      </c>
+      <c r="K26" s="3">
+        <v>148</v>
+      </c>
+      <c r="L26" s="3">
+        <v>162</v>
+      </c>
+      <c r="M26" s="3">
+        <v>176</v>
+      </c>
+      <c r="N26" s="3">
+        <v>190</v>
+      </c>
+      <c r="O26" s="2">
+        <v>204</v>
+      </c>
+      <c r="P26" s="2">
+        <v>218</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>232</v>
+      </c>
+      <c r="R26" s="4">
+        <v>246</v>
+      </c>
+      <c r="S26" s="3">
+        <v>260</v>
+      </c>
+      <c r="T26" s="2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>9</v>
+      </c>
+      <c r="B27" s="3">
+        <v>23</v>
+      </c>
+      <c r="C27" s="4">
+        <v>37</v>
+      </c>
+      <c r="D27" s="3">
+        <v>51</v>
+      </c>
+      <c r="E27" s="3">
+        <v>65</v>
+      </c>
+      <c r="F27" s="2">
+        <v>79</v>
+      </c>
+      <c r="G27" s="2">
+        <v>93</v>
+      </c>
+      <c r="H27" s="2">
+        <v>107</v>
+      </c>
+      <c r="I27" s="2">
+        <v>121</v>
+      </c>
+      <c r="J27" s="2">
+        <v>135</v>
+      </c>
+      <c r="K27" s="2">
+        <v>149</v>
+      </c>
+      <c r="L27" s="2">
+        <v>163</v>
+      </c>
+      <c r="M27" s="2">
+        <v>177</v>
+      </c>
+      <c r="N27" s="2">
+        <v>191</v>
+      </c>
+      <c r="O27" s="2">
+        <v>205</v>
+      </c>
+      <c r="P27" s="3">
+        <v>219</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>233</v>
+      </c>
+      <c r="R27" s="4">
+        <v>247</v>
+      </c>
+      <c r="S27" s="3">
+        <v>261</v>
+      </c>
+      <c r="T27" s="2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4">
+        <v>38</v>
+      </c>
+      <c r="D28" s="3">
+        <v>52</v>
+      </c>
+      <c r="E28" s="3">
+        <v>66</v>
+      </c>
+      <c r="F28" s="3">
+        <v>80</v>
+      </c>
+      <c r="G28" s="3">
+        <v>94</v>
+      </c>
+      <c r="H28" s="2">
+        <v>108</v>
+      </c>
+      <c r="I28" s="3">
+        <v>122</v>
+      </c>
+      <c r="J28" s="4">
+        <v>136</v>
+      </c>
+      <c r="K28" s="4">
+        <v>150</v>
+      </c>
+      <c r="L28" s="3">
+        <v>164</v>
+      </c>
+      <c r="M28" s="2">
+        <v>178</v>
+      </c>
+      <c r="N28" s="3">
+        <v>192</v>
+      </c>
+      <c r="O28" s="3">
+        <v>206</v>
+      </c>
+      <c r="P28" s="3">
+        <v>220</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>234</v>
+      </c>
+      <c r="R28" s="4">
+        <v>248</v>
+      </c>
+      <c r="S28" s="3">
+        <v>262</v>
+      </c>
+      <c r="T28" s="2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>11</v>
+      </c>
+      <c r="B29" s="3">
+        <v>25</v>
+      </c>
+      <c r="C29" s="4">
+        <v>39</v>
+      </c>
+      <c r="D29" s="3">
+        <v>53</v>
+      </c>
+      <c r="E29" s="3">
+        <v>67</v>
+      </c>
+      <c r="F29" s="3">
+        <v>81</v>
+      </c>
+      <c r="G29" s="3">
+        <v>95</v>
+      </c>
+      <c r="H29" s="2">
+        <v>109</v>
+      </c>
+      <c r="I29" s="4">
+        <v>123</v>
+      </c>
+      <c r="J29" s="3">
+        <v>137</v>
+      </c>
+      <c r="K29" s="3">
+        <v>151</v>
+      </c>
+      <c r="L29" s="4">
+        <v>165</v>
+      </c>
+      <c r="M29" s="2">
+        <v>179</v>
+      </c>
+      <c r="N29" s="3">
+        <v>193</v>
+      </c>
+      <c r="O29" s="3">
+        <v>207</v>
+      </c>
+      <c r="P29" s="3">
+        <v>221</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>235</v>
+      </c>
+      <c r="R29" s="4">
+        <v>249</v>
+      </c>
+      <c r="S29" s="3">
+        <v>263</v>
+      </c>
+      <c r="T29" s="2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>12</v>
+      </c>
+      <c r="B30" s="3">
+        <v>26</v>
+      </c>
+      <c r="C30" s="4">
+        <v>40</v>
+      </c>
+      <c r="D30" s="4">
+        <v>54</v>
+      </c>
+      <c r="E30" s="4">
+        <v>68</v>
+      </c>
+      <c r="F30" s="3">
+        <v>82</v>
+      </c>
+      <c r="G30" s="3">
+        <v>96</v>
+      </c>
+      <c r="H30" s="2">
+        <v>110</v>
+      </c>
+      <c r="I30" s="4">
+        <v>124</v>
+      </c>
+      <c r="J30" s="3">
+        <v>138</v>
+      </c>
+      <c r="K30" s="3">
+        <v>152</v>
+      </c>
+      <c r="L30" s="4">
+        <v>166</v>
+      </c>
+      <c r="M30" s="2">
+        <v>180</v>
+      </c>
+      <c r="N30" s="3">
+        <v>194</v>
+      </c>
+      <c r="O30" s="3">
+        <v>208</v>
+      </c>
+      <c r="P30" s="4">
+        <v>222</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>236</v>
+      </c>
+      <c r="R30" s="4">
+        <v>250</v>
+      </c>
+      <c r="S30" s="3">
+        <v>264</v>
+      </c>
+      <c r="T30" s="2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>13</v>
+      </c>
+      <c r="B31" s="3">
+        <v>27</v>
+      </c>
+      <c r="C31" s="3">
+        <v>41</v>
+      </c>
+      <c r="D31" s="3">
+        <v>55</v>
+      </c>
+      <c r="E31" s="3">
+        <v>69</v>
+      </c>
+      <c r="F31" s="3">
+        <v>83</v>
+      </c>
+      <c r="G31" s="3">
+        <v>97</v>
+      </c>
+      <c r="H31" s="2">
+        <v>111</v>
+      </c>
+      <c r="I31" s="3">
+        <v>125</v>
+      </c>
+      <c r="J31" s="4">
+        <v>139</v>
+      </c>
+      <c r="K31" s="4">
+        <v>153</v>
+      </c>
+      <c r="L31" s="3">
+        <v>167</v>
+      </c>
+      <c r="M31" s="2">
+        <v>181</v>
+      </c>
+      <c r="N31" s="3">
+        <v>195</v>
+      </c>
+      <c r="O31" s="3">
+        <v>209</v>
+      </c>
+      <c r="P31" s="3">
+        <v>223</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>237</v>
+      </c>
+      <c r="R31" s="3">
+        <v>251</v>
+      </c>
+      <c r="S31" s="3">
+        <v>265</v>
+      </c>
+      <c r="T31" s="2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>14</v>
+      </c>
+      <c r="B32" s="2">
+        <v>28</v>
+      </c>
+      <c r="C32" s="2">
+        <v>42</v>
+      </c>
+      <c r="D32" s="2">
+        <v>56</v>
+      </c>
+      <c r="E32" s="2">
+        <v>70</v>
+      </c>
+      <c r="F32" s="2">
+        <v>84</v>
+      </c>
+      <c r="G32" s="2">
+        <v>98</v>
+      </c>
+      <c r="H32" s="2">
+        <v>112</v>
+      </c>
+      <c r="I32" s="2">
+        <v>126</v>
+      </c>
+      <c r="J32" s="2">
+        <v>140</v>
+      </c>
+      <c r="K32" s="2">
+        <v>154</v>
+      </c>
+      <c r="L32" s="2">
+        <v>168</v>
+      </c>
+      <c r="M32" s="2">
+        <v>182</v>
+      </c>
+      <c r="N32" s="2">
+        <v>196</v>
+      </c>
+      <c r="O32" s="2">
+        <v>210</v>
+      </c>
+      <c r="P32" s="2">
+        <v>224</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>238</v>
+      </c>
+      <c r="R32" s="2">
+        <v>252</v>
+      </c>
+      <c r="S32" s="2">
+        <v>266</v>
+      </c>
+      <c r="T32" s="2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="33" spans="22:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="22:22" x14ac:dyDescent="0.25">
+      <c r="V36" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>